<commit_message>
Refactor Invoice Creation Logic: Simplify the invoice creation process by consolidating data preparation and removing the update functionality. Enhance the handling of invoice data and line items, ensuring a more streamlined user experience when creating invoices.
</commit_message>
<xml_diff>
--- a/data/Invoices.xlsx
+++ b/data/Invoices.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -533,16 +533,63 @@
       <c r="L3" t="str">
         <v>Net 7</v>
       </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
       <c r="N3" t="str">
         <v>2025-10-30T16:49:53.497Z</v>
       </c>
       <c r="O3" t="str">
         <v>9194b2d3-dacb-4b03-acbc-7e984c1d9afa</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>57fe89c5-a399-4dd1-9830-f513fc466f73</v>
+      </c>
+      <c r="B4" t="str">
+        <v>INV-0001</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2025-10-30</v>
+      </c>
+      <c r="D4" t="str">
+        <v>draft</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>99</v>
+      </c>
+      <c r="G4">
+        <v>8.91</v>
+      </c>
+      <c r="H4">
+        <v>8.91</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>116.82</v>
+      </c>
+      <c r="K4" t="str">
+        <v>chggd</v>
+      </c>
+      <c r="L4" t="str">
+        <v>fdhd</v>
+      </c>
+      <c r="N4" t="str">
+        <v>2025-10-30T17:10:28.233Z</v>
+      </c>
+      <c r="O4" t="str">
+        <v>8bf76e3c-b758-48c5-972a-bb86edf041ec</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>